<commit_message>
Test report is verified for correct data. Test report file removed after testing is finished.
</commit_message>
<xml_diff>
--- a/src/test/resources/example.xlsx
+++ b/src/test/resources/example.xlsx
@@ -7,9 +7,9 @@
     <workbookView xWindow="360" yWindow="75" windowWidth="13395" windowHeight="10545"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" refMode="R1C1"/>
 </workbook>
@@ -548,7 +548,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>